<commit_message>
doc(work logs) : Update
Modified the last comment to make more sense.
</commit_message>
<xml_diff>
--- a/T_CraftMeUp_NeoDarbellay.xlsx
+++ b/T_CraftMeUp_NeoDarbellay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01Modules\02Deuxieme_Annee\P_Prod\Trimestre_2\Craft-Me-Up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575913D0-3C5C-42B3-9A37-38CEF8E0265B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FCC174-B955-4C60-A66F-8D276B008D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -239,7 +239,7 @@
     <t>Continuing code optimization</t>
   </si>
   <si>
-    <t>Progress has been reset as the power got shut down by a classmate</t>
+    <t>All progress here has been reset as the PC's power source got turned off by a classmate.</t>
   </si>
 </sst>
 </file>
@@ -539,6 +539,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -551,40 +568,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1010,10 +1010,10 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1033,65 +1033,65 @@
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="31" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="32"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="33" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="31" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="32"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="36"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1120,7 +1120,7 @@
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="31">
         <v>45964</v>
       </c>
       <c r="C6" s="5">
@@ -1143,7 +1143,7 @@
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="7">
         <v>35</v>
       </c>
@@ -1162,7 +1162,7 @@
       <c r="A8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="27"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="7">
         <v>60</v>
       </c>
@@ -1189,19 +1189,19 @@
       <c r="C9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="26">
         <f>SUM(C6:C8)</f>
         <v>125</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="31">
         <v>45965</v>
       </c>
       <c r="C10" s="5">
@@ -1222,7 +1222,7 @@
       <c r="A11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="27"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="7">
         <v>50</v>
       </c>
@@ -1243,7 +1243,7 @@
       <c r="A12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="27"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="7">
         <v>25</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="A13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="27"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="7">
         <v>35</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="A14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="9">
         <v>35</v>
       </c>
@@ -1310,19 +1310,19 @@
       <c r="C15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="26">
         <f>SUM(C10:C14)</f>
         <v>175</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="31">
         <v>45971</v>
       </c>
       <c r="C16" s="5">
@@ -1345,7 +1345,7 @@
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="27"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="7">
         <v>55</v>
       </c>
@@ -1362,11 +1362,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="27"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="7">
         <v>45</v>
       </c>
@@ -1379,50 +1379,50 @@
       <c r="F18" s="23">
         <v>0.66319444444444442</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="9"/>
+    <row r="19" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="26">
+        <f>SUM(C16:C18)</f>
+        <v>145</v>
+      </c>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
+    </row>
+    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="19"/>
     </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="37">
-        <f>SUM(C16:C20)</f>
-        <v>145</v>
-      </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
+    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="5"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="22"/>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="27"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="27"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="27"/>
+      <c r="B25" s="32"/>
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
-      <c r="B26" s="28"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="9"/>
       <c r="D26" s="8"/>
       <c r="E26" s="10"/>
@@ -1474,17 +1474,17 @@
       <c r="C27" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="37">
-        <f>SUM(C22:C26)</f>
+      <c r="D27" s="26">
+        <f>SUM(C20:C26)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="26"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="5"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="27"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="27"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="27"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="32" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
-      <c r="B32" s="28"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="9"/>
       <c r="D32" s="8"/>
       <c r="E32" s="10"/>
@@ -1537,17 +1537,17 @@
       <c r="C33" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="37">
+      <c r="D33" s="26">
         <f>SUM(C28:C32)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="38"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="26"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="5"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="27"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="7"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="27"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
-      <c r="B37" s="27"/>
+      <c r="B37" s="32"/>
       <c r="C37" s="7"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="38" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
-      <c r="B38" s="28"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="9"/>
       <c r="D38" s="8"/>
       <c r="E38" s="10"/>
@@ -1600,17 +1600,17 @@
       <c r="C39" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="37">
+      <c r="D39" s="26">
         <f>SUM(C34:C38)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="38"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="27"/>
     </row>
     <row r="40" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="26"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="5"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="41" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="27"/>
+      <c r="B41" s="32"/>
       <c r="C41" s="7"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="27"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="7"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="43" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="27"/>
+      <c r="B43" s="32"/>
       <c r="C43" s="7"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="44" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
-      <c r="B44" s="28"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="9"/>
       <c r="D44" s="8"/>
       <c r="E44" s="10"/>
@@ -1663,17 +1663,17 @@
       <c r="C45" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="37">
+      <c r="D45" s="26">
         <f>SUM(C40:C44)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="38"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="26"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="5"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
@@ -1682,7 +1682,7 @@
     </row>
     <row r="47" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
-      <c r="B47" s="27"/>
+      <c r="B47" s="32"/>
       <c r="C47" s="7"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="48" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
-      <c r="B48" s="27"/>
+      <c r="B48" s="32"/>
       <c r="C48" s="7"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="49" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
-      <c r="B49" s="27"/>
+      <c r="B49" s="32"/>
       <c r="C49" s="7"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -1709,7 +1709,7 @@
     </row>
     <row r="50" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9"/>
-      <c r="B50" s="28"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="9"/>
       <c r="D50" s="8"/>
       <c r="E50" s="10"/>
@@ -1726,19 +1726,19 @@
       <c r="C51" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="37">
+      <c r="D51" s="26">
         <f>SUM(C46:C50)</f>
         <v>0</v>
       </c>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="38"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="27"/>
     </row>
     <row r="52" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="30"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="12">
         <f>MROUND(SUM(C6:C51) /60,0.2)</f>
         <v>7.4</v>
@@ -1758,18 +1758,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="B46:B50"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
@@ -1779,18 +1773,24 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D51:G51"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C46:C50 C34:C38 C40:C44 C16:C20 B6 C10:C14 C22:C26 C28:C32 C6:C8" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C46:C50 C34:C38 C40:C44 C16:C18 B6 C10:C14 C20:C26 C28:C32 C6:C8" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B10:B14 B16:B20 B22:B26 B28:B32 B34:B38 B40:B44 B46:B50" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B10:B14 B16:B18 B20:B26 B28:B32 B34:B38 B40:B44 B46:B50" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -1819,7 +1819,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E8 A10:E14 A16:E20 A22:E26 A28:E32 A34:E38 A40:E44 A46:E50 A52:E1048576 A1:D2 F1:F3 A3 D3 G4:G5 G7:G8 A9:D9 A15:D15 A21:D21 A27:D27 A33:D33 A39:D39 A45:D45 A51:D51 G52:G1048576</xm:sqref>
+          <xm:sqref>A4:E8 A10:E14 A16:E18 A20:E26 A28:E32 A34:E38 A40:E44 A46:E50 A52:E1048576 A1:D2 F1:F3 A3 D3 G4:G5 G7:G8 A9:D9 A15:D15 A19:D19 A27:D27 A33:D33 A39:D39 A45:D45 A51:D51 G52:G1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="14" operator="equal" id="{9C6C644F-7238-453A-BC69-B42FAB3A2FA5}">
@@ -1852,7 +1852,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4:E8 E10:E14 E16:E20 E22:E26 E28:E32 E34:E38 E40:E44 E46:E50 E52:E1048576</xm:sqref>
+          <xm:sqref>E4:E8 E10:E14 E16:E18 E20:E26 E28:E32 E34:E38 E40:E44 E46:E50 E52:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="11" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
@@ -1880,7 +1880,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F16:F17 F18:G20</xm:sqref>
+          <xm:sqref>F16:F18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="10" operator="containsText" id="{88417B48-EA26-4D48-9EFE-B6A1E5C426AE}">
@@ -1898,7 +1898,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="8" operator="containsText" id="{756A584A-6AAC-4559-9F27-A59B4EFD7F34}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F22)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F20)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1908,7 +1908,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F22:G26</xm:sqref>
+          <xm:sqref>F20:G26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="7" operator="containsText" id="{E988FD75-2909-4816-91C7-1018002A435D}">
@@ -2003,7 +2003,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G16:G17</xm:sqref>
+          <xm:sqref>G16:G18</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2013,7 +2013,7 @@
           <x14:formula1>
             <xm:f>Restrictions!$A$1:$D$1</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E4 E6:E8 E10:E14 E16:E20 E22:E26 E28:E32 E34:E38 E40:E44 E46:E50 E52:E1048576</xm:sqref>
+          <xm:sqref>E1:E4 E6:E8 E10:E14 E16:E18 E20:E26 E28:E32 E34:E38 E40:E44 E46:E50 E52:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2049,6 +2049,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2291,27 +2311,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2328,23 +2347,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(work log): Updated log
</commit_message>
<xml_diff>
--- a/T_CraftMeUp_NeoDarbellay.xlsx
+++ b/T_CraftMeUp_NeoDarbellay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01Modules\02Deuxieme_Annee\P_Prod\Trimestre_2\Craft-Me-Up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36734FCB-9680-48F9-9E2F-8ADDE1847C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CCB610-5C9D-499F-A0F9-395543B3848E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Restrictions" sheetId="19" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$43</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -264,6 +264,22 @@
   </si>
   <si>
     <t>Still needs some fixing</t>
+  </si>
+  <si>
+    <t>Fixing rendering issues with the new system</t>
+  </si>
+  <si>
+    <t>Fixing projectiles with the new system</t>
+  </si>
+  <si>
+    <t>Since the optimization was so big, a lot of things broke and had to be changed
+There are still some issues, but I'll need Jonathan to help out</t>
+  </si>
+  <si>
+    <t>They shoot again, but have some issues that will need more fixing</t>
+  </si>
+  <si>
+    <t>Re-adding health bar visuals (obstacle, characters)</t>
   </si>
 </sst>
 </file>
@@ -563,6 +579,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -571,51 +623,22 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1052,13 +1075,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1078,65 +1101,65 @@
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="34" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="35"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="36" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="34" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="35"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="28" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="30"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="30"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1165,7 +1188,7 @@
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="26">
         <v>45964</v>
       </c>
       <c r="C6" s="5">
@@ -1188,7 +1211,7 @@
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="7">
         <v>35</v>
       </c>
@@ -1207,7 +1230,7 @@
       <c r="A8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="7">
         <v>60</v>
       </c>
@@ -1234,19 +1257,19 @@
       <c r="C9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="37">
         <f>SUM(C6:C8)</f>
         <v>125</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="26">
         <v>45965</v>
       </c>
       <c r="C10" s="5">
@@ -1267,7 +1290,7 @@
       <c r="A11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="32"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="7">
         <v>50</v>
       </c>
@@ -1288,7 +1311,7 @@
       <c r="A12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="32"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="7">
         <v>25</v>
       </c>
@@ -1309,7 +1332,7 @@
       <c r="A13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="32"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="7">
         <v>35</v>
       </c>
@@ -1328,7 +1351,7 @@
       <c r="A14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="33"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="9">
         <v>35</v>
       </c>
@@ -1355,19 +1378,19 @@
       <c r="C15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="37">
         <f>SUM(C10:C14)</f>
         <v>175</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="26">
         <v>45971</v>
       </c>
       <c r="C16" s="5">
@@ -1390,7 +1413,7 @@
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="32"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="7">
         <v>55</v>
       </c>
@@ -1411,7 +1434,7 @@
       <c r="A18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="32"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="7">
         <v>45</v>
       </c>
@@ -1438,19 +1461,19 @@
       <c r="C19" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="37">
         <f>SUM(C16:C18)</f>
         <v>145</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="27"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="38"/>
     </row>
     <row r="20" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="26">
         <v>45972</v>
       </c>
       <c r="C20" s="5"/>
@@ -1471,7 +1494,7 @@
       <c r="A21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="32"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="7">
         <v>105</v>
       </c>
@@ -1498,19 +1521,19 @@
       <c r="C22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="37">
         <f>SUM(C20:C21)</f>
         <v>105</v>
       </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="38"/>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="26">
         <v>45978</v>
       </c>
       <c r="C23" s="5">
@@ -1533,7 +1556,7 @@
       <c r="A24" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="32"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="7">
         <v>10</v>
       </c>
@@ -1552,7 +1575,7 @@
       <c r="A25" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="32"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="9">
         <v>25</v>
       </c>
@@ -1579,233 +1602,257 @@
       <c r="C26" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="37">
         <f>SUM(C23:C25)</f>
         <v>140</v>
       </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="27"/>
-    </row>
-    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="19"/>
-    </row>
-    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="19"/>
-    </row>
-    <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="7"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="38"/>
+    </row>
+    <row r="27" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="26">
+        <v>45979</v>
+      </c>
+      <c r="C27" s="5">
+        <v>100</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="23">
+        <v>0.4375</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="7">
+        <v>45</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="23">
+        <v>0.46875</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="7">
+        <v>10</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0.47569444444444442</v>
+      </c>
       <c r="G29" s="19"/>
     </row>
-    <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="19"/>
-    </row>
-    <row r="31" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="9"/>
+    <row r="30" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="37">
+        <f>SUM(C27:C29)</f>
+        <v>155</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="38"/>
+    </row>
+    <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="22"/>
       <c r="G31" s="19"/>
     </row>
-    <row r="32" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="26">
-        <f>SUM(C27:C31)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="27"/>
+    <row r="32" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="19"/>
     </row>
     <row r="33" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="5"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="7"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="22"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="19"/>
     </row>
     <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="32"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="7"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="22"/>
+      <c r="F34" s="7"/>
       <c r="G34" s="19"/>
     </row>
-    <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="7"/>
+    <row r="35" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="9"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="E35" s="10"/>
       <c r="F35" s="7"/>
       <c r="G35" s="19"/>
     </row>
-    <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="19"/>
-    </row>
-    <row r="37" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="9"/>
+    <row r="36" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="37">
+        <f>SUM(C31:C35)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="38"/>
+    </row>
+    <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="5"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="7"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="19"/>
     </row>
-    <row r="38" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="26">
-        <f>SUM(C33:C37)</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="27"/>
+    <row r="38" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="19"/>
     </row>
     <row r="39" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="5"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="22"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="19"/>
     </row>
     <row r="40" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
-      <c r="B40" s="32"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="7"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="22"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="19"/>
     </row>
-    <row r="41" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="7"/>
+    <row r="41" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="9"/>
       <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+      <c r="E41" s="10"/>
       <c r="F41" s="7"/>
       <c r="G41" s="19"/>
     </row>
-    <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="19"/>
-    </row>
-    <row r="43" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="19"/>
-    </row>
-    <row r="44" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
+    <row r="42" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B42" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C42" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="26">
-        <f>SUM(C39:C43)</f>
+      <c r="D42" s="37">
+        <f>SUM(C37:C41)</f>
         <v>0</v>
       </c>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="27"/>
-    </row>
-    <row r="45" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="38" t="s">
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="38"/>
+    </row>
+    <row r="43" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="39"/>
-      <c r="C45" s="12">
-        <f>MROUND(SUM(C6:C44) /60,0.2)</f>
-        <v>11.600000000000001</v>
-      </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="14"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="B43" s="30"/>
+      <c r="C43" s="12">
+        <f>MROUND(SUM(C6:C42) /60,0.2)</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
@@ -1815,24 +1862,18 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B37:B41"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C39:C43 C27:C31 C33:C37 C16:C18 B6 C10:C14 C20:C21 C6:C8 C23:C25" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C37:C41 C27:C29 C31:C35 C16:C18 B6 C10:C14 C20:C21 C6:C8 C23:C25" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B10:B14 B16:B18 B20:B21 B39:B43 B27:B31 B33:B37 B23:B25" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B10:B14 B16:B18 B20:B21 B37:B41 B27:B29 B31:B35 B23:B25" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -1851,7 +1892,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="18" operator="equal" id="{6BC2577B-BDA3-4B48-8F95-0F2177F9264F}">
+          <x14:cfRule type="cellIs" priority="19" operator="equal" id="{6BC2577B-BDA3-4B48-8F95-0F2177F9264F}">
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1861,10 +1902,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E8 A10:E14 A16:E18 A20:E21 A27:E31 A33:E37 A39:E43 A45:E1048576 A1:D2 F1:F3 A3 D3 G4:G5 G7:G8 A9:D9 A15:D15 A19:D19 A22:D22 A26:D26 A32:D32 A38:D38 A44:D44 G45:G1048576 A23:E25</xm:sqref>
+          <xm:sqref>A4:E8 A10:E14 A16:E18 A20:E21 A23:E25 A31:E35 A37:E41 A43:E1048576 A1:D2 F1:F3 A3 D3 G4:G5 G7:G8 A9:D9 A15:D15 A19:D19 A22:D22 A26:D26 A30:D30 A36:D36 A42:D42 G43:G1048576 A27:E29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="17" operator="equal" id="{9C6C644F-7238-453A-BC69-B42FAB3A2FA5}">
+          <x14:cfRule type="cellIs" priority="18" operator="equal" id="{9C6C644F-7238-453A-BC69-B42FAB3A2FA5}">
             <xm:f>Restrictions!$A$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1874,7 +1915,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="19" operator="equal" id="{6DE85145-1CAE-407F-B647-4C9B303613C7}">
+          <x14:cfRule type="cellIs" priority="20" operator="equal" id="{6DE85145-1CAE-407F-B647-4C9B303613C7}">
             <xm:f>Restrictions!$C$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1884,7 +1925,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="20" operator="equal" id="{29EA468D-F98D-4D41-AA55-B63DA0941363}">
+          <x14:cfRule type="cellIs" priority="21" operator="equal" id="{29EA468D-F98D-4D41-AA55-B63DA0941363}">
             <xm:f>Restrictions!$D$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1894,10 +1935,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4:E8 E10:E14 E16:E18 E20:E21 E27:E31 E33:E37 E39:E43 E45:E1048576 E23:E25</xm:sqref>
+          <xm:sqref>E4:E8 E10:E14 E16:E18 E20:E21 E23:E25 E27:E29 E31:E35 E37:E41 E43:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F6)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1911,7 +1952,7 @@
           <xm:sqref>F6:F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{6407061A-B268-44CE-A52C-133739941B16}">
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{6407061A-B268-44CE-A52C-133739941B16}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F16)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1925,7 +1966,7 @@
           <xm:sqref>F16:F18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{756A584A-6AAC-4559-9F27-A59B4EFD7F34}">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{756A584A-6AAC-4559-9F27-A59B4EFD7F34}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F20)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1939,7 +1980,21 @@
           <xm:sqref>F20:F21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{88417B48-EA26-4D48-9EFE-B6A1E5C426AE}">
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{E988FD75-2909-4816-91C7-1018002A435D}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F23)))</xm:f>
+            <xm:f>Restrictions!$B$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B0F0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F23 F24:G24 F25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{88417B48-EA26-4D48-9EFE-B6A1E5C426AE}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F10)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1953,21 +2008,7 @@
           <xm:sqref>F10:G10 F11:F12 F13:G13 F14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{E988FD75-2909-4816-91C7-1018002A435D}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F23)))</xm:f>
-            <xm:f>Restrictions!$B$1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF00B0F0"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F23 F24:G24 F25</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{D5B6D5DF-9E2A-4C4B-BA82-97D983766AEE}">
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{D5B6D5DF-9E2A-4C4B-BA82-97D983766AEE}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F27)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1978,11 +2019,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F27:G31</xm:sqref>
+          <xm:sqref>F29:G29 F27:F28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F33)))</xm:f>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F31)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1992,11 +2033,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F33:G37</xm:sqref>
+          <xm:sqref>F31:G35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F39)))</xm:f>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F37)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2006,10 +2047,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F39:G43</xm:sqref>
+          <xm:sqref>F37:G41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{C81CB296-EBDE-4E68-996A-22E647E300C9}">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{C81CB296-EBDE-4E68-996A-22E647E300C9}">
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2022,7 +2063,7 @@
           <xm:sqref>G11:G12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{C6523CE4-984A-4BEA-B850-BBE212DEC1BD}">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{C6523CE4-984A-4BEA-B850-BBE212DEC1BD}">
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2035,7 +2076,7 @@
           <xm:sqref>G14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{34CA0963-7227-4B81-A491-AF5EBF6948E0}">
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{34CA0963-7227-4B81-A491-AF5EBF6948E0}">
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2048,7 +2089,7 @@
           <xm:sqref>G16:G18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{0137ED0B-0223-4A2D-BBA6-66B7E7B0177B}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{0137ED0B-0223-4A2D-BBA6-66B7E7B0177B}">
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2061,7 +2102,7 @@
           <xm:sqref>G20:G21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{0559BE0C-06E8-4BF0-855B-46B347A65A43}">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{0559BE0C-06E8-4BF0-855B-46B347A65A43}">
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2074,7 +2115,7 @@
           <xm:sqref>G23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{A10A680C-18B8-4576-98EE-F30E41E55578}">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{A10A680C-18B8-4576-98EE-F30E41E55578}">
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2086,6 +2127,19 @@
           </x14:cfRule>
           <xm:sqref>G25</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{EE200D4C-87A3-41C0-AADC-DBA0F1BBC7B2}">
+            <xm:f>Restrictions!$B$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B0F0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G27:G28</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -2094,7 +2148,7 @@
           <x14:formula1>
             <xm:f>Restrictions!$A$1:$D$1</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E4 E6:E8 E10:E14 E16:E18 E20:E21 E45:E1048576 E27:E31 E33:E37 E39:E43 E23:E25</xm:sqref>
+          <xm:sqref>E1:E4 E6:E8 E10:E14 E16:E18 E20:E21 E43:E1048576 E27:E29 E31:E35 E37:E41 E23:E25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2130,26 +2184,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2392,10 +2426,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2412,20 +2477,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>